<commit_message>
Agrega punto decimal en escalado, y vista reactor
</commit_message>
<xml_diff>
--- a/documentation/ordenRegistrosReactor.xlsx
+++ b/documentation/ordenRegistrosReactor.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -446,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
       <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>

</xml_diff>